<commit_message>
converting URIs into w3id.org/italia/controlled-vocabulary for chanel and interactivity-level  controlled vocabularies and inserted German translations; fix minor typo in authentication controlled vocabulary
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-public-services/channel/channel.xlsx
+++ b/VocabolariControllati/classifications-for-public-services/channel/channel.xlsx
@@ -19,19 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
-  <si>
-    <t>Codice 1 livello</t>
-  </si>
-  <si>
-    <t>Label 1 Livello</t>
-  </si>
-  <si>
-    <t>Codice 2 livello</t>
-  </si>
-  <si>
-    <t>Label 2 livello</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="150">
   <si>
     <t>01</t>
   </si>
@@ -42,57 +30,27 @@
     <t>01.1</t>
   </si>
   <si>
-    <t>Diretto</t>
-  </si>
-  <si>
-    <t>Codice 3 livello</t>
-  </si>
-  <si>
     <t>01.1.1</t>
   </si>
   <si>
-    <t>Label 3 livello</t>
-  </si>
-  <si>
-    <t>sportello PA</t>
-  </si>
-  <si>
     <t>01.1.2</t>
   </si>
   <si>
-    <t>domicilio cittadino</t>
-  </si>
-  <si>
     <t>01.1.3</t>
   </si>
   <si>
-    <t>cassa automatica</t>
-  </si>
-  <si>
     <t>01.2</t>
   </si>
   <si>
-    <t>Con intermediario</t>
-  </si>
-  <si>
     <t>01.2.1</t>
   </si>
   <si>
-    <t>posta</t>
-  </si>
-  <si>
     <t>01.2.2</t>
   </si>
   <si>
-    <t>tabaccaio/ricevitoria</t>
-  </si>
-  <si>
     <t>01.2.3</t>
   </si>
   <si>
-    <t>GDO</t>
-  </si>
-  <si>
     <t>01.2.4</t>
   </si>
   <si>
@@ -102,9 +60,6 @@
     <t>01.2.5</t>
   </si>
   <si>
-    <t>altri intermediari</t>
-  </si>
-  <si>
     <t>02</t>
   </si>
   <si>
@@ -204,21 +159,12 @@
     <t>05.5.1</t>
   </si>
   <si>
-    <t>pagamento in tempo reale</t>
-  </si>
-  <si>
     <t>05.5.2</t>
   </si>
   <si>
-    <t>incasso preautorizzato</t>
-  </si>
-  <si>
     <t>05.5.3</t>
   </si>
   <si>
-    <t>pagamento attivo presso PSP (Prestatore di Servizio di Pagamento)</t>
-  </si>
-  <si>
     <t>05.6</t>
   </si>
   <si>
@@ -228,15 +174,9 @@
     <t>05.6.1</t>
   </si>
   <si>
-    <t>ordine permanente</t>
-  </si>
-  <si>
     <t>05.6.2</t>
   </si>
   <si>
-    <t>addebito diretto / SEPA</t>
-  </si>
-  <si>
     <t>05.6.3</t>
   </si>
   <si>
@@ -259,18 +199,289 @@
   </si>
   <si>
     <t>F23</t>
+  </si>
+  <si>
+    <t>Non-electronic</t>
+  </si>
+  <si>
+    <t>Nicht Telematisch</t>
+  </si>
+  <si>
+    <t>Non telematico diretto</t>
+  </si>
+  <si>
+    <t>Direct non-electronic</t>
+  </si>
+  <si>
+    <t>Nicht-direkte Telematik</t>
+  </si>
+  <si>
+    <t>Sportello Pubblica Amministrazione</t>
+  </si>
+  <si>
+    <t>Public Administration information desk</t>
+  </si>
+  <si>
+    <t>Informationsstelle der öffentlichen Verwaltung</t>
+  </si>
+  <si>
+    <t>Domicilio del cittadino</t>
+  </si>
+  <si>
+    <t>Citizen residence</t>
+  </si>
+  <si>
+    <t>Wohnsitz des Bürgers</t>
+  </si>
+  <si>
+    <t>Cassa automatica</t>
+  </si>
+  <si>
+    <t>Paymnet machine</t>
+  </si>
+  <si>
+    <t>Automatische Kasse</t>
+  </si>
+  <si>
+    <t>Non telematico con intermediario</t>
+  </si>
+  <si>
+    <t>Direct non-electronic with mediator</t>
+  </si>
+  <si>
+    <t>Nicht telematisch mit Vermittler</t>
+  </si>
+  <si>
+    <t>Posta</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Tabaccaio - Ricevitoria</t>
+  </si>
+  <si>
+    <t>Tobacco shop - box office</t>
+  </si>
+  <si>
+    <t>Tabakladen - Abendkasse</t>
+  </si>
+  <si>
+    <t>GDO - Grande Distribuzione Organizzata</t>
+  </si>
+  <si>
+    <t>Large scale distribution</t>
+  </si>
+  <si>
+    <t>Organisierter Großvertrieb</t>
+  </si>
+  <si>
+    <t>Assistance Centre</t>
+  </si>
+  <si>
+    <t>Assistenzzentrum</t>
+  </si>
+  <si>
+    <t>Altro intermediario</t>
+  </si>
+  <si>
+    <t>Other mediator</t>
+  </si>
+  <si>
+    <t>Sonstiger Vermittler</t>
+  </si>
+  <si>
+    <t>Web Site</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Free Online Form</t>
+  </si>
+  <si>
+    <t>Online-Formular nicht ausgefüllt</t>
+  </si>
+  <si>
+    <t>Pre-filled Online Form</t>
+  </si>
+  <si>
+    <t>Vorkompiliertes Online-Modul</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Telefon</t>
+  </si>
+  <si>
+    <t>Voice</t>
+  </si>
+  <si>
+    <t>Dedizierte Nummer/Stimme</t>
+  </si>
+  <si>
+    <t>Call Center</t>
+  </si>
+  <si>
+    <t>E-Mail</t>
+  </si>
+  <si>
+    <t>Certified Electronic Mail</t>
+  </si>
+  <si>
+    <t>Zertifizierte elektronische Post - PEC</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Other electronic</t>
+  </si>
+  <si>
+    <t>Sonstige Telematik</t>
+  </si>
+  <si>
+    <t>App mobile</t>
+  </si>
+  <si>
+    <t>Mobile Anwendung</t>
+  </si>
+  <si>
+    <t>TV auf Abruf</t>
+  </si>
+  <si>
+    <t>Computer kiosk</t>
+  </si>
+  <si>
+    <t>Video conferencing</t>
+  </si>
+  <si>
+    <t>Videokonferenz</t>
+  </si>
+  <si>
+    <t>PagoPA Platform</t>
+  </si>
+  <si>
+    <t>PagoPA-Plattform</t>
+  </si>
+  <si>
+    <t>Pagamento in tempo reale</t>
+  </si>
+  <si>
+    <t>Real time payment</t>
+  </si>
+  <si>
+    <t>Echtzeit-Zahlung</t>
+  </si>
+  <si>
+    <t>Incasso preautorizzato</t>
+  </si>
+  <si>
+    <t>Pre-authorised payment</t>
+  </si>
+  <si>
+    <t>Vorautorisierte Zahlung</t>
+  </si>
+  <si>
+    <t>Pagamento attivo presso PSP - Prestatore di Servizio di Pagamento</t>
+  </si>
+  <si>
+    <t>Payment carried out through Service Payment Provider</t>
+  </si>
+  <si>
+    <t>Zahlung erfolgt über Service Payment Provider</t>
+  </si>
+  <si>
+    <t>Automated bank payment</t>
+  </si>
+  <si>
+    <t>Automatische Banküberweisungen</t>
+  </si>
+  <si>
+    <t>Ordine permanente</t>
+  </si>
+  <si>
+    <t>Standing order</t>
+  </si>
+  <si>
+    <t>Dauerauftrag</t>
+  </si>
+  <si>
+    <t>Addebito diretto - SEPA</t>
+  </si>
+  <si>
+    <t>Direct debit</t>
+  </si>
+  <si>
+    <t>Direktabbuchung</t>
+  </si>
+  <si>
+    <t>Bank transfer</t>
+  </si>
+  <si>
+    <t>Banküberweisung</t>
+  </si>
+  <si>
+    <t>Payment against notice</t>
+  </si>
+  <si>
+    <t>Zahlung gegen Mahnung</t>
+  </si>
+  <si>
+    <t>Paymnet form F24</t>
+  </si>
+  <si>
+    <t>Payment form F23</t>
+  </si>
+  <si>
+    <t>codice_1_livello</t>
+  </si>
+  <si>
+    <t>label_ITA_1_livello</t>
+  </si>
+  <si>
+    <t>label_ENG_1_livello</t>
+  </si>
+  <si>
+    <t>label_DEU_1_livello</t>
+  </si>
+  <si>
+    <t>codice _2_livello</t>
+  </si>
+  <si>
+    <t>label_ITA_2_livello</t>
+  </si>
+  <si>
+    <t>label_ENG_2_livello</t>
+  </si>
+  <si>
+    <t>label_DEU_2_livello</t>
+  </si>
+  <si>
+    <t>codice_3_livello</t>
+  </si>
+  <si>
+    <t>Label_ITA_3_livello</t>
+  </si>
+  <si>
+    <t>label_ENG_3_livello</t>
+  </si>
+  <si>
+    <t>label_DEU_3_livello</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -297,6 +508,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -366,7 +590,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -380,6 +604,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
@@ -759,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:B29"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -773,538 +1002,1011 @@
     <col min="4" max="4" width="40.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
     <col min="6" max="6" width="42.5" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:12">
       <c r="A1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="J8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="J9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="C10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="F10" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="G10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F11" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="F12" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="F13" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="F14" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="5" t="s">
+      <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="F15" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" t="s">
+        <v>103</v>
+      </c>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="F16" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="F17" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="s">
+      <c r="H17" t="s">
+        <v>108</v>
+      </c>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="5" t="s">
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" t="s">
+        <v>109</v>
+      </c>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C19" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="5" t="s">
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="5" t="s">
+      <c r="F20" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="G20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" t="s">
+        <v>112</v>
+      </c>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="F21" t="s">
         <v>44</v>
       </c>
-      <c r="D15" t="s">
+      <c r="G21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="J21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K21" t="s">
+        <v>116</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="F22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" t="s">
+        <v>114</v>
+      </c>
+      <c r="I22" t="s">
         <v>46</v>
       </c>
-      <c r="D16" t="s">
+      <c r="J22" t="s">
+        <v>118</v>
+      </c>
+      <c r="K22" t="s">
+        <v>119</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I23" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="5" t="s">
+      <c r="J23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K23" t="s">
+        <v>122</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="F24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="G24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I24" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s">
+      <c r="J24" t="s">
+        <v>126</v>
+      </c>
+      <c r="K24" t="s">
+        <v>127</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="5" t="s">
+      <c r="J25" t="s">
+        <v>129</v>
+      </c>
+      <c r="K25" t="s">
+        <v>130</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="G26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D18" t="s">
+      <c r="J26" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="5" t="s">
+      <c r="K26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L26" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="G27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D19" t="s">
+      <c r="J27" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="5" t="s">
+      <c r="K27" t="s">
+        <v>134</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="G28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D20" t="s">
+      <c r="J28" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="5" t="s">
+      <c r="K28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="G29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D21" t="s">
+      <c r="J29" t="s">
         <v>59</v>
       </c>
-      <c r="E21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="K29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L29" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E22" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="5"/>
       <c r="B30" s="1"/>
       <c r="C30" s="3"/>
       <c r="D30" s="1"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:12">
       <c r="A31" s="5"/>
       <c r="B31" s="1"/>
       <c r="C31" s="3"/>
       <c r="D31" s="1"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:12">
       <c r="A32" s="5"/>
       <c r="B32" s="1"/>
       <c r="C32" s="3"/>

</xml_diff>

<commit_message>
upload new version 0.2 of channel controlled vocabulary. The versionInfo metadata indicates the single changes that were applied
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-public-services/channel/channel.xlsx
+++ b/VocabolariControllati/classifications-for-public-services/channel/channel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="150">
   <si>
     <t>01</t>
   </si>
@@ -63,21 +63,12 @@
     <t>02</t>
   </si>
   <si>
-    <t>Sito Web</t>
-  </si>
-  <si>
     <t>02.1</t>
   </si>
   <si>
-    <t>Modulo online libero</t>
-  </si>
-  <si>
     <t>02.2</t>
   </si>
   <si>
-    <t>Modulo online precompilato</t>
-  </si>
-  <si>
     <t>03</t>
   </si>
   <si>
@@ -291,21 +282,9 @@
     <t>Sonstiger Vermittler</t>
   </si>
   <si>
-    <t>Web Site</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>Free Online Form</t>
-  </si>
-  <si>
     <t>Online-Formular nicht ausgefüllt</t>
   </si>
   <si>
-    <t>Pre-filled Online Form</t>
-  </si>
-  <si>
     <t>Vorkompiliertes Online-Modul</t>
   </si>
   <si>
@@ -469,6 +448,27 @@
   </si>
   <si>
     <t>label_DEU_3_livello</t>
+  </si>
+  <si>
+    <t>Applicativo</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Applikation</t>
+  </si>
+  <si>
+    <t>Applicazione con compilazione modulo libero</t>
+  </si>
+  <si>
+    <t>Applicazione con modulo precompilato</t>
+  </si>
+  <si>
+    <t>Application with pre-filled form</t>
+  </si>
+  <si>
+    <t>Application with free form</t>
   </si>
 </sst>
 </file>
@@ -539,8 +539,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -610,7 +614,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="53">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
@@ -635,6 +639,8 @@
     <cellStyle name="Collegamento ipertestuale" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
@@ -659,6 +665,8 @@
     <cellStyle name="Collegamento visitato" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -988,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1012,40 +1020,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1056,34 +1064,34 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1094,34 +1102,34 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1132,34 +1140,34 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1170,34 +1178,34 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1208,34 +1216,34 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1246,34 +1254,34 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1284,22 +1292,22 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>10</v>
@@ -1308,10 +1316,10 @@
         <v>11</v>
       </c>
       <c r="K8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1322,34 +1330,34 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1357,25 +1365,25 @@
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>146</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="H10" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="L10" s="8"/>
     </row>
@@ -1384,634 +1392,667 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>147</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>94</v>
+        <v>148</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J12" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="7"/>
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H13" t="s">
-        <v>100</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="7"/>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="7"/>
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="H15" t="s">
-        <v>103</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="J15" s="1"/>
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="H16" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>106</v>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>107</v>
+        <v>23</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="H17" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="L17" s="8"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>105</v>
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="H18" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>105</v>
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" t="s">
-        <v>110</v>
+        <v>29</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="H19" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="L19" s="8"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="H20" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="F21" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>113</v>
+        <v>35</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
       </c>
       <c r="H21" t="s">
-        <v>114</v>
-      </c>
-      <c r="I21" t="s">
-        <v>45</v>
-      </c>
-      <c r="J21" t="s">
-        <v>115</v>
-      </c>
-      <c r="K21" t="s">
-        <v>116</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>117</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="L21" s="8"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>113</v>
+        <v>37</v>
+      </c>
+      <c r="G22" t="s">
+        <v>103</v>
       </c>
       <c r="H22" t="s">
-        <v>114</v>
-      </c>
-      <c r="I22" t="s">
-        <v>46</v>
-      </c>
-      <c r="J22" t="s">
-        <v>118</v>
-      </c>
-      <c r="K22" t="s">
-        <v>119</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>120</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="L22" s="8"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" t="s">
-        <v>44</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H23" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" t="s">
-        <v>47</v>
-      </c>
-      <c r="J23" t="s">
-        <v>121</v>
-      </c>
-      <c r="K23" t="s">
-        <v>122</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>123</v>
-      </c>
+      <c r="L23" s="8"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>125</v>
+      <c r="H24" t="s">
+        <v>107</v>
       </c>
       <c r="I24" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J24" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="K24" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>51</v>
+      <c r="H25" t="s">
+        <v>107</v>
+      </c>
+      <c r="I25" t="s">
+        <v>43</v>
       </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="K25" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>52</v>
+      <c r="H26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" t="s">
+        <v>44</v>
       </c>
       <c r="J26" t="s">
-        <v>53</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>132</v>
+        <v>114</v>
+      </c>
+      <c r="K26" t="s">
+        <v>115</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>54</v>
+        <v>118</v>
+      </c>
+      <c r="I27" t="s">
+        <v>47</v>
       </c>
       <c r="J27" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="K27" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="J28" t="s">
+        <v>122</v>
+      </c>
+      <c r="K28" t="s">
+        <v>123</v>
+      </c>
+      <c r="L28" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" t="s">
-        <v>57</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="L28" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H29" s="1" t="s">
+      <c r="J29" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J29" t="s">
-        <v>59</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="L29" s="9" t="s">
-        <v>59</v>
+      <c r="L29" s="8" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="5"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="3"/>
+      <c r="A30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J30" t="s">
+        <v>52</v>
+      </c>
+      <c r="K30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="5"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="3"/>
+      <c r="A31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J31" t="s">
+        <v>54</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="5"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="3"/>
+      <c r="A32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" t="s">
+        <v>56</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5"/>
@@ -2022,17 +2063,38 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5"/>
-      <c r="B34" s="3"/>
+      <c r="B34" s="1"/>
       <c r="C34" s="3"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="5"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="5"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="5"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="5"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
uploaded version 0.2 of Atlas of Paths ontology; updated channels.xlsx
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-public-services/channel/channel.xlsx
+++ b/VocabolariControllati/classifications-for-public-services/channel/channel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="158">
   <si>
     <t>01</t>
   </si>
@@ -156,39 +156,18 @@
     <t>05.5.3</t>
   </si>
   <si>
-    <t>05.6</t>
-  </si>
-  <si>
     <t>Pagamenti bancari automatici</t>
   </si>
   <si>
-    <t>05.6.1</t>
-  </si>
-  <si>
-    <t>05.6.2</t>
-  </si>
-  <si>
-    <t>05.6.3</t>
-  </si>
-  <si>
     <t>Bonifico</t>
   </si>
   <si>
-    <t>05.6.4</t>
-  </si>
-  <si>
     <t>MAV/RAV</t>
   </si>
   <si>
-    <t>05.6.5</t>
-  </si>
-  <si>
     <t>F24</t>
   </si>
   <si>
-    <t>05.6.6</t>
-  </si>
-  <si>
     <t>F23</t>
   </si>
   <si>
@@ -282,12 +261,6 @@
     <t>Sonstiger Vermittler</t>
   </si>
   <si>
-    <t>Online-Formular nicht ausgefüllt</t>
-  </si>
-  <si>
-    <t>Vorkompiliertes Online-Modul</t>
-  </si>
-  <si>
     <t>Telephone</t>
   </si>
   <si>
@@ -456,19 +429,70 @@
     <t>Application</t>
   </si>
   <si>
-    <t>Applikation</t>
-  </si>
-  <si>
     <t>Applicazione con compilazione modulo libero</t>
   </si>
   <si>
     <t>Applicazione con modulo precompilato</t>
   </si>
   <si>
-    <t>Application with pre-filled form</t>
-  </si>
-  <si>
-    <t>Application with free form</t>
+    <t>Softwareapplikation mit formular nicht ausgefüllt</t>
+  </si>
+  <si>
+    <t>Softwareapplikation mit vorkompiliertes Modul</t>
+  </si>
+  <si>
+    <t>Softwareapplikation</t>
+  </si>
+  <si>
+    <t>Software application with free form</t>
+  </si>
+  <si>
+    <t>Software application with pre-filled form</t>
+  </si>
+  <si>
+    <t>02.3</t>
+  </si>
+  <si>
+    <t>Applicazione Web</t>
+  </si>
+  <si>
+    <t>02.4</t>
+  </si>
+  <si>
+    <t>02.5</t>
+  </si>
+  <si>
+    <t>Applicazione Desktop</t>
+  </si>
+  <si>
+    <t>Web Application</t>
+  </si>
+  <si>
+    <t>Desktop Application</t>
+  </si>
+  <si>
+    <t>Web-Applikation</t>
+  </si>
+  <si>
+    <t>Desktop-Applikation</t>
+  </si>
+  <si>
+    <t>05.4.1</t>
+  </si>
+  <si>
+    <t>05.4.2</t>
+  </si>
+  <si>
+    <t>05.4.3</t>
+  </si>
+  <si>
+    <t>05.5.4</t>
+  </si>
+  <si>
+    <t>05.5.5</t>
+  </si>
+  <si>
+    <t>05.5.6</t>
   </si>
 </sst>
 </file>
@@ -539,8 +563,84 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -614,7 +714,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="129">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
@@ -641,6 +741,44 @@
     <cellStyle name="Collegamento ipertestuale" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
@@ -667,6 +805,44 @@
     <cellStyle name="Collegamento visitato" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -996,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1011,7 +1187,7 @@
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
     <col min="6" max="6" width="42.5" customWidth="1"/>
     <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="55.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="46" bestFit="1" customWidth="1"/>
@@ -1020,40 +1196,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1064,34 +1240,34 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1102,34 +1278,34 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="K3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1140,34 +1316,34 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1178,34 +1354,34 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1216,34 +1392,34 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1254,34 +1430,34 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="K7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1292,22 +1468,22 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>10</v>
@@ -1316,10 +1492,10 @@
         <v>11</v>
       </c>
       <c r="K8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1330,34 +1506,34 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1365,25 +1541,25 @@
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="H10" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="L10" s="8"/>
     </row>
@@ -1392,25 +1568,25 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="L11" s="8"/>
     </row>
@@ -1419,17 +1595,26 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>150</v>
+      </c>
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12">
@@ -1437,17 +1622,26 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="7"/>
+      <c r="F13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H13" t="s">
+        <v>151</v>
+      </c>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12">
@@ -1455,17 +1649,26 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="7"/>
+        <v>140</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
+        <v>92</v>
+      </c>
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12">
@@ -1476,10 +1679,10 @@
         <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>18</v>
@@ -1488,10 +1691,10 @@
         <v>19</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H15" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="J15" s="1"/>
       <c r="L15" s="8"/>
@@ -1504,10 +1707,10 @@
         <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>20</v>
@@ -1516,10 +1719,10 @@
         <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="L16" s="8"/>
     </row>
@@ -1531,10 +1734,10 @@
         <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>22</v>
@@ -1561,7 +1764,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>26</v>
@@ -1570,10 +1773,10 @@
         <v>27</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H18" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="L18" s="8"/>
     </row>
@@ -1588,7 +1791,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>28</v>
@@ -1597,10 +1800,10 @@
         <v>29</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H19" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="L19" s="8"/>
     </row>
@@ -1608,26 +1811,26 @@
       <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G20" t="s">
+        <v>35</v>
       </c>
       <c r="H20" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="L20" s="8"/>
     </row>
@@ -1639,22 +1842,22 @@
         <v>31</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="H21" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="L21" s="8"/>
     </row>
@@ -1666,22 +1869,22 @@
         <v>31</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>36</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
-      </c>
-      <c r="G22" t="s">
-        <v>103</v>
+        <v>39</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="H22" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="L22" s="8"/>
     </row>
@@ -1693,24 +1896,35 @@
         <v>31</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="I23" t="s">
+        <v>152</v>
+      </c>
+      <c r="J23" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H23" t="s">
-        <v>105</v>
-      </c>
-      <c r="L23" s="8"/>
+      <c r="K23" t="s">
+        <v>100</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="5" t="s">
@@ -1720,34 +1934,34 @@
         <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F24" t="s">
         <v>41</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="H24" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I24" t="s">
-        <v>42</v>
+        <v>153</v>
       </c>
       <c r="J24" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K24" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1758,34 +1972,34 @@
         <v>31</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F25" t="s">
         <v>41</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" t="s">
+        <v>154</v>
+      </c>
+      <c r="J25" t="s">
+        <v>105</v>
+      </c>
+      <c r="K25" t="s">
         <v>106</v>
       </c>
-      <c r="H25" t="s">
+      <c r="L25" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="I25" t="s">
-        <v>43</v>
-      </c>
-      <c r="J25" t="s">
-        <v>111</v>
-      </c>
-      <c r="K25" t="s">
-        <v>112</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1796,34 +2010,34 @@
         <v>31</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F26" t="s">
-        <v>41</v>
+      <c r="F26" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H26" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="I26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J26" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K26" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1834,34 +2048,34 @@
         <v>31</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I27" t="s">
-        <v>47</v>
+        <v>109</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="J27" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K27" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1872,34 +2086,34 @@
         <v>31</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J28" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="K28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L28" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J28" t="s">
-        <v>122</v>
-      </c>
-      <c r="K28" t="s">
-        <v>123</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1910,34 +2124,34 @@
         <v>31</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="G29" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="H29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J29" t="s">
+        <v>47</v>
+      </c>
+      <c r="K29" t="s">
         <v>118</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J29" t="s">
-        <v>50</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="L29" s="8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1948,34 +2162,34 @@
         <v>31</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="G30" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
       <c r="J30" t="s">
-        <v>52</v>
-      </c>
-      <c r="K30" t="s">
-        <v>127</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>128</v>
+        <v>48</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1986,73 +2200,42 @@
         <v>31</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="G31" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>53</v>
+        <v>157</v>
       </c>
       <c r="J31" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J32" t="s">
-        <v>56</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="L32" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="A32" s="5"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5"/>
@@ -2077,24 +2260,17 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="5"/>
-      <c r="B36" s="1"/>
+      <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="5"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="5"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="5"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>